<commit_message>
Static scenario analysis - cascade plots
</commit_message>
<xml_diff>
--- a/model/static/Static Scenarios.xlsx
+++ b/model/static/Static Scenarios.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adenooy/Library/CloudStorage/OneDrive-Personal/UVA/Thesis/MSc-Thesis/model/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ae90f5cbd0fd171/UVA/Thesis/MSc-Thesis/model/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126412A1-FC3C-6943-A7EC-D18FA39CAA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{126412A1-FC3C-6943-A7EC-D18FA39CAA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{822B40A6-3CB2-F243-A93B-67797383F2DD}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="960" windowWidth="27640" windowHeight="15640" xr2:uid="{FE4CE163-9160-A349-872A-020A306ED76D}"/>
   </bookViews>
@@ -143,13 +143,13 @@
     <t>Everyone receives a decentralised swab-based GeneXert and gets result in same visit</t>
   </si>
   <si>
-    <t>A greater number of correct results are generated. Further, all sites have testing capapcity, hence fewer people are lost from care  as a result of needing to attend another facility. Oral swab will allow for all individuals to provide a sample (particulalry HIV+) and increase ease and likelihood of testing being offered</t>
-  </si>
-  <si>
-    <t>Testing occurs fully with GeneXpert, as opposed to a proportion with smear microscopy, hence a greater number of correct results will be generated. Oral swab will allow for all individuals to provide a sample (particulalry HIV+)  and increase ease and likelihood of testing being offered</t>
-  </si>
-  <si>
-    <t>A greater number of correct results are generated. All sites have testing capapcity, hence fewer people are lost from care as a result of needing to attend another facility. All results are availble at the time of testing and a subsequent visit to collect results is not required. Oral swab will allow for all individuals to provide a sample (particulalry HIV+)  and increase ease and likelihood of testing being offered</t>
+    <t>Testing occurs fully with GeneXpert, as opposed to a proportion with smear microscopy, hence a greater number of correct results will be generated. Oral swab will allow for all individuals to provide a sample (particularly HIV+)  and increase ease and likelihood of testing being offered</t>
+  </si>
+  <si>
+    <t>A greater number of correct results are generated. Further, all sites have testing capapcity, hence fewer people are lost from care  as a result of needing to attend another facility. Oral swab will allow for all individuals to provide a sample (particularly HIV+) and increase ease and likelihood of testing being offered</t>
+  </si>
+  <si>
+    <t>A greater number of correct results are generated. All sites have testing capapcity, hence fewer people are lost from care as a result of needing to attend another facility. All results are availble at the time of testing and a subsequent visit to collect results is not required. Oral swab will allow for all individuals to provide a sample (particularly HIV+)  and increase ease and likelihood of testing being offered</t>
   </si>
 </sst>
 </file>
@@ -537,33 +537,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046C2023-CCAB-8643-8533-96999460350E}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="62.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="39.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="40.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -573,20 +575,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -596,20 +598,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -619,20 +621,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -642,20 +644,20 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -665,66 +667,66 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="238" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="147" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -757,13 +759,13 @@
       <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -780,13 +782,13 @@
       <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="1" t="s">

</xml_diff>